<commit_message>
started working on noise simulation in Hybrid Jobs looking into pulse_level calibrations accessing default calibrations from hardware providers it looks like estimating expectation values needs to be handled by the user - goal: build own Estimator primitive
</commit_message>
<xml_diff>
--- a/00_AWS/aws_braket_cost_calculator.xlsx
+++ b/00_AWS/aws_braket_cost_calculator.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasvoss/Documents/Master Wirtschaftsphysik/Masterarbeit Yale-NUS CQT/Quantum_Optimal_Control/00_AWS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258AB8E9-EF62-FB45-B3FF-CC2105895736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994574B9-0037-E64C-95D4-850AA9038820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{4C9EA9AD-6C95-804B-AA8A-FDC273B842CA}"/>
+    <workbookView xWindow="1780" yWindow="1240" windowWidth="28040" windowHeight="17440" xr2:uid="{4C9EA9AD-6C95-804B-AA8A-FDC273B842CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -465,7 +465,7 @@
   <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="186" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,13 +504,13 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>500</v>
+        <v>160</v>
       </c>
       <c r="C8">
-        <v>300</v>
+        <v>130</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="E8">
         <v>9</v>
@@ -543,7 +543,7 @@
       </c>
       <c r="E13" s="3">
         <f>PRODUCT($B$8,$C$8,$E$8)*($C13+PRODUCT($D$8,$D13))</f>
-        <v>405472.5</v>
+        <v>64022.399999999994</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -558,7 +558,7 @@
       </c>
       <c r="E14" s="3">
         <f>PRODUCT($B$8,$C$8,$E$8)*($C14+PRODUCT($D$8,$D14))</f>
-        <v>405472.5</v>
+        <v>64022.399999999994</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
@@ -572,8 +572,8 @@
         <v>0.01</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" ref="E14:E15" si="0">PRODUCT($B$8,$C$8,$E$8)*($C15+PRODUCT($D$8,$D15))</f>
-        <v>418500</v>
+        <f t="shared" ref="E15" si="0">PRODUCT($B$8,$C$8,$E$8)*($C15+PRODUCT($D$8,$D15))</f>
+        <v>280800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor aws folder and draft AWSEstimator
* Folder 04_hybrid_jobs had a subfolder in which all files were
now removed that submolder with files being in 04 directly

* Draft of an AWSEstimator class to measure scaled sums of pauli observables
</commit_message>
<xml_diff>
--- a/00_AWS/aws_braket_cost_calculator.xlsx
+++ b/00_AWS/aws_braket_cost_calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasvoss/Documents/Master Wirtschaftsphysik/Masterarbeit Yale-NUS CQT/Quantum_Optimal_Control/00_AWS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994574B9-0037-E64C-95D4-850AA9038820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173CC2F0-B322-5745-9402-71D336523C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="1240" windowWidth="28040" windowHeight="17440" xr2:uid="{4C9EA9AD-6C95-804B-AA8A-FDC273B842CA}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="186" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,13 +504,13 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="C8">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D8">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="E8">
         <v>9</v>
@@ -543,7 +543,7 @@
       </c>
       <c r="E13" s="3">
         <f>PRODUCT($B$8,$C$8,$E$8)*($C13+PRODUCT($D$8,$D13))</f>
-        <v>64022.399999999994</v>
+        <v>96228</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -558,7 +558,7 @@
       </c>
       <c r="E14" s="3">
         <f>PRODUCT($B$8,$C$8,$E$8)*($C14+PRODUCT($D$8,$D14))</f>
-        <v>64022.399999999994</v>
+        <v>96228</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
@@ -573,7 +573,7 @@
       </c>
       <c r="E15" s="3">
         <f t="shared" ref="E15" si="0">PRODUCT($B$8,$C$8,$E$8)*($C15+PRODUCT($D$8,$D15))</f>
-        <v>280800</v>
+        <v>784080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>